<commit_message>
Apache read from excel and build object functional, dropdown on label setup is still pending.
</commit_message>
<xml_diff>
--- a/test-input/Label.xlsx
+++ b/test-input/Label.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\IdeaProjects\LabelSetup\test-input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Intellij\LabelSetup\test-input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,12 +29,6 @@
     <t>CAMPBELL</t>
   </si>
   <si>
-    <t>Label Format</t>
-  </si>
-  <si>
-    <t>LabelType</t>
-  </si>
-  <si>
     <t>Outbound Customer Case Label</t>
   </si>
   <si>
@@ -42,6 +36,12 @@
   </si>
   <si>
     <t>GORTON1</t>
+  </si>
+  <si>
+    <t>labelForm</t>
+  </si>
+  <si>
+    <t>labelType</t>
   </si>
 </sst>
 </file>
@@ -375,18 +375,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -394,23 +392,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>